<commit_message>
Refactoring and test fixes
Refactor interaction with form controls a little
Add common atomic value parser, remove per-type value parsers
Refactor class parser
Add custom exceptions
Do some small todos
Fix typo
Add/fix some tests
</commit_message>
<xml_diff>
--- a/Files/importAfterCreate_template.xlsx
+++ b/Files/importAfterCreate_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Ценовой лист</t>
   </si>
@@ -32,12 +32,6 @@
   </si>
   <si>
     <t>Value::Type</t>
-  </si>
-  <si>
-    <t>Value::Items[].Id</t>
-  </si>
-  <si>
-    <t>Value::Items[].Name</t>
   </si>
   <si>
     <t>CheckBox:CheckBoxName1:TestFlag1</t>
@@ -952,7 +946,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,13 +1082,13 @@
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="60"/>
       <c r="G8" s="60"/>
       <c r="H8" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1161,12 +1155,8 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>7</v>
-      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="23"/>

</xml_diff>